<commit_message>
Titles, axis, space, comments, etc for plots
</commit_message>
<xml_diff>
--- a/Data/regression_data/Population/regression_Population.xlsx
+++ b/Data/regression_data/Population/regression_Population.xlsx
@@ -450,7 +450,7 @@
         <v>1600</v>
       </c>
       <c r="B2" t="n">
-        <v>397832.5576969567</v>
+        <v>397832.5590765636</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1601</v>
       </c>
       <c r="B3" t="n">
-        <v>398296.4280610727</v>
+        <v>398296.4294421462</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>1602</v>
       </c>
       <c r="B4" t="n">
-        <v>398766.9480888849</v>
+        <v>398766.9494714359</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>1603</v>
       </c>
       <c r="B5" t="n">
-        <v>399244.2122193377</v>
+        <v>399244.2136033769</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>1604</v>
       </c>
       <c r="B6" t="n">
-        <v>399728.3162069325</v>
+        <v>399728.3175924707</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>1605</v>
       </c>
       <c r="B7" t="n">
-        <v>400219.3571393072</v>
+        <v>400219.3585263552</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>1606</v>
       </c>
       <c r="B8" t="n">
-        <v>400717.4334550301</v>
+        <v>400717.4348435986</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>1607</v>
       </c>
       <c r="B9" t="n">
-        <v>401222.6449616064</v>
+        <v>401222.6463517063</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>1608</v>
       </c>
       <c r="B10" t="n">
-        <v>401735.0928537041</v>
+        <v>401735.0942453461</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>1609</v>
       </c>
       <c r="B11" t="n">
-        <v>402254.8797315969</v>
+        <v>402254.8811247918</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>1610</v>
       </c>
       <c r="B12" t="n">
-        <v>402782.1096198286</v>
+        <v>402782.1110145871</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>1611</v>
       </c>
       <c r="B13" t="n">
-        <v>403316.8879860999</v>
+        <v>403316.8893824328</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>1612</v>
       </c>
       <c r="B14" t="n">
-        <v>403859.3217603796</v>
+        <v>403859.3231582976</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>1613</v>
       </c>
       <c r="B15" t="n">
-        <v>404409.5193542427</v>
+        <v>404409.5207537565</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>1614</v>
       </c>
       <c r="B16" t="n">
-        <v>404967.5906804359</v>
+        <v>404967.5920815563</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>1615</v>
       </c>
       <c r="B17" t="n">
-        <v>405533.6471726741</v>
+        <v>405533.6485754117</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>1616</v>
       </c>
       <c r="B18" t="n">
-        <v>406107.8018056682</v>
+        <v>406107.8032100335</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>1617</v>
       </c>
       <c r="B19" t="n">
-        <v>406690.1691153867</v>
+        <v>406690.1705213905</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>1618</v>
       </c>
       <c r="B20" t="n">
-        <v>407280.8652195541</v>
+        <v>407280.8666272069</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>1619</v>
       </c>
       <c r="B21" t="n">
-        <v>407880.0078383848</v>
+        <v>407880.0092476972</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>1620</v>
       </c>
       <c r="B22" t="n">
-        <v>408487.7163155579</v>
+        <v>408487.7177265403</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>1621</v>
       </c>
       <c r="B23" t="n">
-        <v>409104.1116394321</v>
+        <v>409104.113052095</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>1622</v>
       </c>
       <c r="B24" t="n">
-        <v>409729.3164645036</v>
+        <v>409729.3178788575</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>1623</v>
       </c>
       <c r="B25" t="n">
-        <v>410363.4551331087</v>
+        <v>410363.4565491638</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>1624</v>
       </c>
       <c r="B26" t="n">
-        <v>411006.6536973718</v>
+        <v>411006.6551151386</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>1625</v>
       </c>
       <c r="B27" t="n">
-        <v>411659.0399414027</v>
+        <v>411659.0413608913</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>1626</v>
       </c>
       <c r="B28" t="n">
-        <v>412320.7434037414</v>
+        <v>412320.7448249621</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>1627</v>
       </c>
       <c r="B29" t="n">
-        <v>412991.8954000561</v>
+        <v>412991.8968230191</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>1628</v>
       </c>
       <c r="B30" t="n">
-        <v>413672.6290460925</v>
+        <v>413672.6304708078</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>1629</v>
       </c>
       <c r="B31" t="n">
-        <v>414363.079280878</v>
+        <v>414363.0807073556</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1630</v>
       </c>
       <c r="B32" t="n">
-        <v>415063.3828901814</v>
+        <v>415063.3843184313</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1631</v>
       </c>
       <c r="B33" t="n">
-        <v>415773.6785302307</v>
+        <v>415773.6799602626</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1632</v>
       </c>
       <c r="B34" t="n">
-        <v>416494.1067516881</v>
+        <v>416494.1081835119</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1633</v>
       </c>
       <c r="B35" t="n">
-        <v>417224.8100238873</v>
+        <v>417224.8114575126</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1634</v>
       </c>
       <c r="B36" t="n">
-        <v>417965.9327593303</v>
+        <v>417965.9341947667</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1635</v>
       </c>
       <c r="B37" t="n">
-        <v>418717.6213384487</v>
+        <v>418717.6227757058</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1636</v>
       </c>
       <c r="B38" t="n">
-        <v>419480.0241346282</v>
+        <v>419480.0255737154</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1637</v>
       </c>
       <c r="B39" t="n">
-        <v>420253.291539499</v>
+        <v>420253.2929804255</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1638</v>
       </c>
       <c r="B40" t="n">
-        <v>421037.5759884923</v>
+        <v>421037.5774312675</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1639</v>
       </c>
       <c r="B41" t="n">
-        <v>421833.0319866658</v>
+        <v>421833.0334312984</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1640</v>
       </c>
       <c r="B42" t="n">
-        <v>422639.8161347958</v>
+        <v>422639.817581295</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1641</v>
       </c>
       <c r="B43" t="n">
-        <v>423458.0871557416</v>
+        <v>423458.0886041162</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1642</v>
       </c>
       <c r="B44" t="n">
-        <v>424288.0059210789</v>
+        <v>424288.0073713376</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1643</v>
       </c>
       <c r="B45" t="n">
-        <v>425129.7354780058</v>
+        <v>425129.7369301571</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1644</v>
       </c>
       <c r="B46" t="n">
-        <v>425983.4410765209</v>
+        <v>425983.4425305732</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1645</v>
       </c>
       <c r="B47" t="n">
-        <v>426849.2901968748</v>
+        <v>426849.2916528364</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1646</v>
       </c>
       <c r="B48" t="n">
-        <v>427727.4525772957</v>
+        <v>427727.4540351748</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1647</v>
       </c>
       <c r="B49" t="n">
-        <v>428618.1002419893</v>
+        <v>428618.1017017938</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1648</v>
       </c>
       <c r="B50" t="n">
-        <v>429521.4075294138</v>
+        <v>429521.4089911515</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1649</v>
       </c>
       <c r="B51" t="n">
-        <v>430437.5511208308</v>
+        <v>430437.5525845094</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1650</v>
       </c>
       <c r="B52" t="n">
-        <v>431366.7100691316</v>
+        <v>431366.7115347585</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1651</v>
       </c>
       <c r="B53" t="n">
-        <v>432309.0658279402</v>
+        <v>432309.0672955227</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1652</v>
       </c>
       <c r="B54" t="n">
-        <v>433264.802280992</v>
+        <v>433264.8037505372</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1653</v>
       </c>
       <c r="B55" t="n">
-        <v>434234.1057717896</v>
+        <v>434234.1072433044</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1654</v>
       </c>
       <c r="B56" t="n">
-        <v>435217.1651335346</v>
+        <v>435217.1666070256</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1655</v>
       </c>
       <c r="B57" t="n">
-        <v>436214.1717193355</v>
+        <v>436214.1731948093</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1656</v>
       </c>
       <c r="B58" t="n">
-        <v>437225.3194326927</v>
+        <v>437225.3209101555</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1657</v>
       </c>
       <c r="B59" t="n">
-        <v>438250.8047582578</v>
+        <v>438250.8062377158</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1658</v>
       </c>
       <c r="B60" t="n">
-        <v>439290.8267928693</v>
+        <v>439290.8282743281</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1659</v>
       </c>
       <c r="B61" t="n">
-        <v>440345.5872768621</v>
+        <v>440345.5887603274</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>1660</v>
       </c>
       <c r="B62" t="n">
-        <v>441415.2906256521</v>
+        <v>441415.2921111293</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>1661</v>
       </c>
       <c r="B63" t="n">
-        <v>442500.1439615925</v>
+        <v>442500.1454490866</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>1662</v>
       </c>
       <c r="B64" t="n">
-        <v>443600.3571461039</v>
+        <v>443600.3586356198</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>1663</v>
       </c>
       <c r="B65" t="n">
-        <v>444716.1428120739</v>
+        <v>444716.1443036161</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>1664</v>
       </c>
       <c r="B66" t="n">
-        <v>445847.7163965279</v>
+        <v>445847.7178901008</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>1665</v>
       </c>
       <c r="B67" t="n">
-        <v>446995.2961735674</v>
+        <v>446995.2976691747</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>1666</v>
       </c>
       <c r="B68" t="n">
-        <v>448159.1032875752</v>
+        <v>448159.1047852209</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>1667</v>
       </c>
       <c r="B69" t="n">
-        <v>449339.3617866869</v>
+        <v>449339.3632863744</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>1668</v>
       </c>
       <c r="B70" t="n">
-        <v>450536.2986565241</v>
+        <v>450536.3001582564</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>1669</v>
       </c>
       <c r="B71" t="n">
-        <v>451750.14385419</v>
+        <v>451750.1453579699</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>1670</v>
       </c>
       <c r="B72" t="n">
-        <v>452981.1303425234</v>
+        <v>452981.1318483533</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>1671</v>
       </c>
       <c r="B73" t="n">
-        <v>454229.4941246096</v>
+        <v>454229.4956324917</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>1672</v>
       </c>
       <c r="B74" t="n">
-        <v>455495.4742785455</v>
+        <v>455495.4757884815</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>1673</v>
       </c>
       <c r="B75" t="n">
-        <v>456779.3129924551</v>
+        <v>456779.3145044465</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>1674</v>
       </c>
       <c r="B76" t="n">
-        <v>458081.2555997545</v>
+        <v>458081.2571138024</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>1675</v>
       </c>
       <c r="B77" t="n">
-        <v>459401.5506146612</v>
+        <v>459401.552130766</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>1676</v>
       </c>
       <c r="B78" t="n">
-        <v>460740.4497679445</v>
+        <v>460740.4512861067</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>1677</v>
       </c>
       <c r="B79" t="n">
-        <v>462098.2080429154</v>
+        <v>462098.2095631349</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>1678</v>
       </c>
       <c r="B80" t="n">
-        <v>463475.0837116496</v>
+        <v>463475.0852339258</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>1679</v>
       </c>
       <c r="B81" t="n">
-        <v>464871.3383714405</v>
+        <v>464871.3398957726</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>1680</v>
       </c>
       <c r="B82" t="n">
-        <v>466287.2369814791</v>
+        <v>466287.2385078656</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>1681</v>
       </c>
       <c r="B83" t="n">
-        <v>467723.0478997533</v>
+        <v>467723.0494281924</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>1682</v>
       </c>
       <c r="B84" t="n">
-        <v>469179.0429201654</v>
+        <v>469179.0444506549</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>1683</v>
       </c>
       <c r="B85" t="n">
-        <v>470655.4973098597</v>
+        <v>470655.4988423969</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>1684</v>
       </c>
       <c r="B86" t="n">
-        <v>472152.6898467565</v>
+        <v>472152.6913813382</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>1685</v>
       </c>
       <c r="B87" t="n">
-        <v>473670.9028572861</v>
+        <v>473670.9043939086</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>1686</v>
       </c>
       <c r="B88" t="n">
-        <v>475210.4222543173</v>
+        <v>475210.4237929765</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>1687</v>
       </c>
       <c r="B89" t="n">
-        <v>476771.5375752744</v>
+        <v>476771.5391159654</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>1688</v>
       </c>
       <c r="B90" t="n">
-        <v>478354.5420204342</v>
+        <v>478354.5435631521</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>1689</v>
       </c>
       <c r="B91" t="n">
-        <v>479959.7324914007</v>
+        <v>479959.7340361397</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>1690</v>
       </c>
       <c r="B92" t="n">
-        <v>481587.4096297444</v>
+        <v>481587.411176498</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>1691</v>
       </c>
       <c r="B93" t="n">
-        <v>483237.8778558029</v>
+        <v>483237.8794045645</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>1692</v>
       </c>
       <c r="B94" t="n">
-        <v>484911.4454076348</v>
+        <v>484911.4469583969</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>1693</v>
       </c>
       <c r="B95" t="n">
-        <v>486608.4243801158</v>
+        <v>486608.4259328704</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>1694</v>
       </c>
       <c r="B96" t="n">
-        <v>488329.1307641717</v>
+        <v>488329.1323189103</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>1695</v>
       </c>
       <c r="B97" t="n">
-        <v>490073.8844861381</v>
+        <v>490073.8860428514</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>1696</v>
       </c>
       <c r="B98" t="n">
-        <v>491843.0094472359</v>
+        <v>491843.0110059141</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>1697</v>
       </c>
       <c r="B99" t="n">
-        <v>493636.8335631571</v>
+        <v>493636.8351237897</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>1698</v>
       </c>
       <c r="B100" t="n">
-        <v>495455.688803746</v>
+        <v>495455.6903663218</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>1699</v>
       </c>
       <c r="B101" t="n">
-        <v>497299.9112327688</v>
+        <v>497299.912797276</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>1700</v>
       </c>
       <c r="B102" t="n">
-        <v>499169.8410477589</v>
+        <v>499169.8426141852</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>1701</v>
       </c>
       <c r="B103" t="n">
-        <v>501065.8226199282</v>
+        <v>501065.8241882601</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>1702</v>
       </c>
       <c r="B104" t="n">
-        <v>502988.2045341298</v>
+        <v>502988.2061043535</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>1703</v>
       </c>
       <c r="B105" t="n">
-        <v>504937.339628864</v>
+        <v>504937.3412009649</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>1704</v>
       </c>
       <c r="B106" t="n">
-        <v>506913.5850363107</v>
+        <v>506913.5866102735</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>1705</v>
       </c>
       <c r="B107" t="n">
-        <v>508917.3022223784</v>
+        <v>508917.3037981869</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>1706</v>
       </c>
       <c r="B108" t="n">
-        <v>510948.8570267539</v>
+        <v>510948.8586043911</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>1707</v>
       </c>
       <c r="B109" t="n">
-        <v>513008.6197029398</v>
+        <v>513008.6212823879</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>1708</v>
       </c>
       <c r="B110" t="n">
-        <v>515096.9649582651</v>
+        <v>515096.9665395056</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>1709</v>
       </c>
       <c r="B111" t="n">
-        <v>517214.2719938528</v>
+        <v>517214.2735768665</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>1710</v>
       </c>
       <c r="B112" t="n">
-        <v>519360.9245445307</v>
+        <v>519360.9261292972</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>1711</v>
       </c>
       <c r="B113" t="n">
-        <v>521537.3109186664</v>
+        <v>521537.3125051646</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>1712</v>
       </c>
       <c r="B114" t="n">
-        <v>523743.8240379125</v>
+        <v>523743.8256261206</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>1713</v>
       </c>
       <c r="B115" t="n">
-        <v>525980.8614768432</v>
+        <v>525980.8630667382</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>1714</v>
       </c>
       <c r="B116" t="n">
-        <v>528248.8255024643</v>
+        <v>528248.8270940225</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>1715</v>
       </c>
       <c r="B117" t="n">
-        <v>530548.1231135782</v>
+        <v>530548.1247067748</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>1716</v>
       </c>
       <c r="B118" t="n">
-        <v>532879.1660799857</v>
+        <v>532879.1676747951</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>1717</v>
       </c>
       <c r="B119" t="n">
-        <v>535242.3709815034</v>
+        <v>535242.372577899</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>1718</v>
       </c>
       <c r="B120" t="n">
-        <v>537638.1592467772</v>
+        <v>537638.1608447314</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>1719</v>
       </c>
       <c r="B121" t="n">
-        <v>540066.9571918703</v>
+        <v>540066.9587913544</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>1720</v>
       </c>
       <c r="B122" t="n">
-        <v>542529.1960586053</v>
+        <v>542529.1976595897</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>1721</v>
       </c>
       <c r="B123" t="n">
-        <v>545025.3120526352</v>
+        <v>545025.3136550891</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>1722</v>
       </c>
       <c r="B124" t="n">
-        <v>547555.7463812242</v>
+        <v>547555.747985116</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>1723</v>
       </c>
       <c r="B125" t="n">
-        <v>550120.9452907105</v>
+        <v>550120.9468960072</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>1724</v>
       </c>
       <c r="B126" t="n">
-        <v>552721.3601036299</v>
+        <v>552721.3617102974</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>1725</v>
       </c>
       <c r="B127" t="n">
-        <v>555357.4472554725</v>
+        <v>555357.4488634759</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>1726</v>
       </c>
       <c r="B128" t="n">
-        <v>558029.6683310483</v>
+        <v>558029.6699403513</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>1727</v>
       </c>
       <c r="B129" t="n">
-        <v>560738.4901004342</v>
+        <v>560738.4917109993</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>1728</v>
       </c>
       <c r="B130" t="n">
-        <v>563484.384554474</v>
+        <v>563484.3861662628</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>1729</v>
       </c>
       <c r="B131" t="n">
-        <v>566267.8289398063</v>
+        <v>566267.8305527789</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>1730</v>
       </c>
       <c r="B132" t="n">
-        <v>569089.3057933862</v>
+        <v>569089.3074075015</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>1731</v>
       </c>
       <c r="B133" t="n">
-        <v>571949.302976476</v>
+        <v>571949.3045916918</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>1732</v>
       </c>
       <c r="B134" t="n">
-        <v>574848.3137080705</v>
+        <v>574848.3153243433</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>1733</v>
       </c>
       <c r="B135" t="n">
-        <v>577786.836597728</v>
+        <v>577786.8382150128</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>1734</v>
       </c>
       <c r="B136" t="n">
-        <v>580765.3756777717</v>
+        <v>580765.3772960225</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>1735</v>
       </c>
       <c r="B137" t="n">
-        <v>583784.4404348314</v>
+        <v>583784.4420540005</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>1736</v>
       </c>
       <c r="B138" t="n">
-        <v>586844.5458406887</v>
+        <v>586844.5474607274</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>1737</v>
       </c>
       <c r="B139" t="n">
-        <v>589946.2123823923</v>
+        <v>589946.21400325</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>1738</v>
       </c>
       <c r="B140" t="n">
-        <v>593089.9660916058</v>
+        <v>593089.9677132313</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>1739</v>
       </c>
       <c r="B141" t="n">
-        <v>596276.3385731548</v>
+        <v>596276.3401954947</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>1740</v>
       </c>
       <c r="B142" t="n">
-        <v>599505.8670327283</v>
+        <v>599505.8686557283</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>1741</v>
       </c>
       <c r="B143" t="n">
-        <v>602779.0943037047</v>
+        <v>602779.0959273088</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>1742</v>
       </c>
       <c r="B144" t="n">
-        <v>606096.568873055</v>
+        <v>606096.5704972056</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>1743</v>
       </c>
       <c r="B145" t="n">
-        <v>609458.844906287</v>
+        <v>609458.846530925</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>1744</v>
       </c>
       <c r="B146" t="n">
-        <v>612866.4822713865</v>
+        <v>612866.4838964515</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>1745</v>
       </c>
       <c r="B147" t="n">
-        <v>616320.0465617146</v>
+        <v>616320.0481871443</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>1746</v>
       </c>
       <c r="B148" t="n">
-        <v>619820.1091178152</v>
+        <v>619820.1107435459</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>1747</v>
       </c>
       <c r="B149" t="n">
-        <v>623367.24704809</v>
+        <v>623367.2486740567</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>1748</v>
       </c>
       <c r="B150" t="n">
-        <v>626962.0432482953</v>
+        <v>626962.0448744309</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>1749</v>
       </c>
       <c r="B151" t="n">
-        <v>630605.0864198105</v>
+        <v>630605.0880460463</v>
       </c>
     </row>
     <row r="152">
@@ -1650,7 +1650,7 @@
         <v>1750</v>
       </c>
       <c r="B152" t="n">
-        <v>634296.9710866355</v>
+        <v>634296.9727129011</v>
       </c>
     </row>
     <row r="153">
@@ -1658,7 +1658,7 @@
         <v>1751</v>
       </c>
       <c r="B153" t="n">
-        <v>638038.2976110632</v>
+        <v>638038.2992372868</v>
       </c>
     </row>
     <row r="154">
@@ -1666,7 +1666,7 @@
         <v>1752</v>
       </c>
       <c r="B154" t="n">
-        <v>641829.6722079822</v>
+        <v>641829.6738340901</v>
       </c>
     </row>
     <row r="155">
@@ -1674,7 +1674,7 @@
         <v>1753</v>
       </c>
       <c r="B155" t="n">
-        <v>645671.7069577533</v>
+        <v>645671.7085836699</v>
       </c>
     </row>
     <row r="156">
@@ -1682,7 +1682,7 @@
         <v>1754</v>
       </c>
       <c r="B156" t="n">
-        <v>649565.019817611</v>
+        <v>649565.0214432592</v>
       </c>
     </row>
     <row r="157">
@@ -1690,7 +1690,7 @@
         <v>1755</v>
       </c>
       <c r="B157" t="n">
-        <v>653510.2346315372</v>
+        <v>653510.2362568378</v>
       </c>
     </row>
     <row r="158">
@@ -1698,7 +1698,7 @@
         <v>1756</v>
       </c>
       <c r="B158" t="n">
-        <v>657507.9811385501</v>
+        <v>657507.9827634224</v>
       </c>
     </row>
     <row r="159">
@@ -1706,7 +1706,7 @@
         <v>1757</v>
       </c>
       <c r="B159" t="n">
-        <v>661558.8949793549</v>
+        <v>661558.8966037163</v>
       </c>
     </row>
     <row r="160">
@@ -1714,7 +1714,7 @@
         <v>1758</v>
       </c>
       <c r="B160" t="n">
-        <v>665663.6177013007</v>
+        <v>665663.6193250662</v>
       </c>
     </row>
     <row r="161">
@@ -1722,7 +1722,7 @@
         <v>1759</v>
       </c>
       <c r="B161" t="n">
-        <v>669822.796761581</v>
+        <v>669822.7983846645</v>
       </c>
     </row>
     <row r="162">
@@ -1730,7 +1730,7 @@
         <v>1760</v>
       </c>
       <c r="B162" t="n">
-        <v>674037.0855286268</v>
+        <v>674037.08715094</v>
       </c>
     </row>
     <row r="163">
@@ -1738,7 +1738,7 @@
         <v>1761</v>
       </c>
       <c r="B163" t="n">
-        <v>678307.1432816257</v>
+        <v>678307.1449030782</v>
       </c>
     </row>
     <row r="164">
@@ -1746,7 +1746,7 @@
         <v>1762</v>
       </c>
       <c r="B164" t="n">
-        <v>682633.6352081094</v>
+        <v>682633.6368286088</v>
       </c>
     </row>
     <row r="165">
@@ -1754,7 +1754,7 @@
         <v>1763</v>
       </c>
       <c r="B165" t="n">
-        <v>687017.2323995461</v>
+        <v>687017.2340189982</v>
       </c>
     </row>
     <row r="166">
@@ -1762,7 +1762,7 @@
         <v>1764</v>
       </c>
       <c r="B166" t="n">
-        <v>691458.6118448756</v>
+        <v>691458.6134631842</v>
       </c>
     </row>
     <row r="167">
@@ -1770,7 +1770,7 @@
         <v>1765</v>
       </c>
       <c r="B167" t="n">
-        <v>695958.4564219229</v>
+        <v>695958.4580389897</v>
       </c>
     </row>
     <row r="168">
@@ -1778,7 +1778,7 @@
         <v>1766</v>
       </c>
       <c r="B168" t="n">
-        <v>700517.4548866235</v>
+        <v>700517.4565023483</v>
       </c>
     </row>
     <row r="169">
@@ -1786,7 +1786,7 @@
         <v>1767</v>
       </c>
       <c r="B169" t="n">
-        <v>705136.3018599952</v>
+        <v>705136.3034742755</v>
       </c>
     </row>
     <row r="170">
@@ -1794,7 +1794,7 @@
         <v>1768</v>
       </c>
       <c r="B170" t="n">
-        <v>709815.697812788</v>
+        <v>709815.6994255192</v>
       </c>
     </row>
     <row r="171">
@@ -1802,7 +1802,7 @@
         <v>1769</v>
       </c>
       <c r="B171" t="n">
-        <v>714556.3490477436</v>
+        <v>714556.3506588193</v>
       </c>
     </row>
     <row r="172">
@@ -1810,7 +1810,7 @@
         <v>1770</v>
       </c>
       <c r="B172" t="n">
-        <v>719358.967679396</v>
+        <v>719358.9692887075</v>
       </c>
     </row>
     <row r="173">
@@ -1818,7 +1818,7 @@
         <v>1771</v>
       </c>
       <c r="B173" t="n">
-        <v>724224.2716113391</v>
+        <v>724224.2732187754</v>
       </c>
     </row>
     <row r="174">
@@ -1826,7 +1826,7 @@
         <v>1772</v>
       </c>
       <c r="B174" t="n">
-        <v>729152.9845108935</v>
+        <v>729152.9861163417</v>
       </c>
     </row>
     <row r="175">
@@ -1834,7 +1834,7 @@
         <v>1773</v>
       </c>
       <c r="B175" t="n">
-        <v>734145.8357810958</v>
+        <v>734145.8373844405</v>
       </c>
     </row>
     <row r="176">
@@ -1842,7 +1842,7 @@
         <v>1774</v>
       </c>
       <c r="B176" t="n">
-        <v>739203.5605299387</v>
+        <v>739203.5621310624</v>
       </c>
     </row>
     <row r="177">
@@ -1850,7 +1850,7 @@
         <v>1775</v>
       </c>
       <c r="B177" t="n">
-        <v>744326.8995367866</v>
+        <v>744326.9011355699</v>
       </c>
     </row>
     <row r="178">
@@ -1858,7 +1858,7 @@
         <v>1776</v>
       </c>
       <c r="B178" t="n">
-        <v>749516.5992158898</v>
+        <v>749516.6008122107</v>
       </c>
     </row>
     <row r="179">
@@ -1866,7 +1866,7 @@
         <v>1777</v>
       </c>
       <c r="B179" t="n">
-        <v>754773.4115769211</v>
+        <v>754773.4131706553</v>
       </c>
     </row>
     <row r="180">
@@ -1874,7 +1874,7 @@
         <v>1778</v>
       </c>
       <c r="B180" t="n">
-        <v>760098.0941824564</v>
+        <v>760098.0957734771</v>
       </c>
     </row>
     <row r="181">
@@ -1882,7 +1882,7 @@
         <v>1779</v>
       </c>
       <c r="B181" t="n">
-        <v>765491.41010232</v>
+        <v>765491.4116904987</v>
       </c>
     </row>
     <row r="182">
@@ -1890,7 +1890,7 @@
         <v>1780</v>
       </c>
       <c r="B182" t="n">
-        <v>770954.1278647176</v>
+        <v>770954.1294499234</v>
       </c>
     </row>
     <row r="183">
@@ -1898,7 +1898,7 @@
         <v>1781</v>
       </c>
       <c r="B183" t="n">
-        <v>776487.0214040722</v>
+        <v>776487.0229861713</v>
       </c>
     </row>
     <row r="184">
@@ -1906,7 +1906,7 @@
         <v>1782</v>
       </c>
       <c r="B184" t="n">
-        <v>782090.8700054837</v>
+        <v>782090.8715843403</v>
       </c>
     </row>
     <row r="185">
@@ -1914,7 +1914,7 @@
         <v>1783</v>
       </c>
       <c r="B185" t="n">
-        <v>787766.4582457305</v>
+        <v>787766.4598212066</v>
       </c>
     </row>
     <row r="186">
@@ -1922,7 +1922,7 @@
         <v>1784</v>
       </c>
       <c r="B186" t="n">
-        <v>793514.5759307293</v>
+        <v>793514.5775026841</v>
       </c>
     </row>
     <row r="187">
@@ -1930,7 +1930,7 @@
         <v>1785</v>
       </c>
       <c r="B187" t="n">
-        <v>799336.0180293673</v>
+        <v>799336.0195976582</v>
       </c>
     </row>
     <row r="188">
@@ -1938,7 +1938,7 @@
         <v>1786</v>
       </c>
       <c r="B188" t="n">
-        <v>805231.5846036284</v>
+        <v>805231.5861681097</v>
       </c>
     </row>
     <row r="189">
@@ -1946,7 +1946,7 @@
         <v>1787</v>
       </c>
       <c r="B189" t="n">
-        <v>811202.0807349187</v>
+        <v>811202.0822954428</v>
       </c>
     </row>
     <row r="190">
@@ -1954,7 +1954,7 @@
         <v>1788</v>
       </c>
       <c r="B190" t="n">
-        <v>817248.3164465157</v>
+        <v>817248.3180029325</v>
       </c>
     </row>
     <row r="191">
@@ -1962,7 +1962,7 @@
         <v>1789</v>
       </c>
       <c r="B191" t="n">
-        <v>823371.1066220482</v>
+        <v>823371.1081742048</v>
       </c>
     </row>
     <row r="192">
@@ -1970,7 +1970,7 @@
         <v>1790</v>
       </c>
       <c r="B192" t="n">
-        <v>829571.2709199213</v>
+        <v>829571.2724676628</v>
       </c>
     </row>
     <row r="193">
@@ -1978,7 +1978,7 @@
         <v>1791</v>
       </c>
       <c r="B193" t="n">
-        <v>835849.6336836031</v>
+        <v>835849.6352267719</v>
       </c>
     </row>
     <row r="194">
@@ -1986,7 +1986,7 @@
         <v>1792</v>
       </c>
       <c r="B194" t="n">
-        <v>842207.0238476794</v>
+        <v>842207.0253861155</v>
       </c>
     </row>
     <row r="195">
@@ -1994,7 +1994,7 @@
         <v>1793</v>
       </c>
       <c r="B195" t="n">
-        <v>848644.2748395933</v>
+        <v>848644.2763731342</v>
       </c>
     </row>
     <row r="196">
@@ -2002,7 +2002,7 @@
         <v>1794</v>
       </c>
       <c r="B196" t="n">
-        <v>855162.2244769793</v>
+        <v>855162.2260054604</v>
       </c>
     </row>
     <row r="197">
@@ -2010,7 +2010,7 @@
         <v>1795</v>
       </c>
       <c r="B197" t="n">
-        <v>861761.7148605051</v>
+        <v>861761.7163837585</v>
       </c>
     </row>
     <row r="198">
@@ -2018,7 +2018,7 @@
         <v>1796</v>
       </c>
       <c r="B198" t="n">
-        <v>868443.5922621294</v>
+        <v>868443.5937799852</v>
       </c>
     </row>
     <row r="199">
@@ -2026,7 +2026,7 @@
         <v>1797</v>
       </c>
       <c r="B199" t="n">
-        <v>875208.7070086913</v>
+        <v>875208.7085209771</v>
       </c>
     </row>
     <row r="200">
@@ -2034,7 +2034,7 @@
         <v>1798</v>
       </c>
       <c r="B200" t="n">
-        <v>882057.9133607398</v>
+        <v>882057.9148672806</v>
       </c>
     </row>
     <row r="201">
@@ -2042,7 +2042,7 @@
         <v>1799</v>
       </c>
       <c r="B201" t="n">
-        <v>888992.0693865151</v>
+        <v>888992.0708871339</v>
       </c>
     </row>
     <row r="202">
@@ -2050,7 +2050,7 @@
         <v>1800</v>
       </c>
       <c r="B202" t="n">
-        <v>896012.0368309971</v>
+        <v>896012.0383255137</v>
       </c>
     </row>
     <row r="203">
@@ -2058,7 +2058,7 @@
         <v>1801</v>
       </c>
       <c r="B203" t="n">
-        <v>903118.6809799264</v>
+        <v>903118.6824681584</v>
       </c>
     </row>
     <row r="204">
@@ -2066,7 +2066,7 @@
         <v>1802</v>
       </c>
       <c r="B204" t="n">
-        <v>910312.870518717</v>
+        <v>910312.8720004798</v>
       </c>
     </row>
     <row r="205">
@@ -2074,7 +2074,7 @@
         <v>1803</v>
       </c>
       <c r="B205" t="n">
-        <v>917595.4773861701</v>
+        <v>917595.4788612761</v>
       </c>
     </row>
     <row r="206">
@@ -2082,7 +2082,7 @@
         <v>1804</v>
       </c>
       <c r="B206" t="n">
-        <v>924967.3766229022</v>
+        <v>924967.3780911621</v>
       </c>
     </row>
     <row r="207">
@@ -2090,7 +2090,7 @@
         <v>1805</v>
       </c>
       <c r="B207" t="n">
-        <v>932429.4462144044</v>
+        <v>932429.4476756258</v>
       </c>
     </row>
     <row r="208">
@@ -2098,7 +2098,7 @@
         <v>1806</v>
       </c>
       <c r="B208" t="n">
-        <v>939982.5669286442</v>
+        <v>939982.568382632</v>
       </c>
     </row>
     <row r="209">
@@ -2106,7 +2106,7 @@
         <v>1807</v>
       </c>
       <c r="B209" t="n">
-        <v>947627.6221481278</v>
+        <v>947627.6235946855</v>
       </c>
     </row>
     <row r="210">
@@ -2114,7 +2114,7 @@
         <v>1808</v>
       </c>
       <c r="B210" t="n">
-        <v>955365.497696341</v>
+        <v>955365.4991352689</v>
       </c>
     </row>
     <row r="211">
@@ -2122,7 +2122,7 @@
         <v>1809</v>
       </c>
       <c r="B211" t="n">
-        <v>963197.0816584828</v>
+        <v>963197.0830895789</v>
       </c>
     </row>
     <row r="212">
@@ -2130,7 +2130,7 @@
         <v>1810</v>
       </c>
       <c r="B212" t="n">
-        <v>971123.264196415</v>
+        <v>971123.2656194749</v>
       </c>
     </row>
     <row r="213">
@@ -2138,7 +2138,7 @@
         <v>1811</v>
       </c>
       <c r="B213" t="n">
-        <v>979144.9373577456</v>
+        <v>979144.9387725629</v>
       </c>
     </row>
     <row r="214">
@@ -2146,7 +2146,7 @@
         <v>1812</v>
       </c>
       <c r="B214" t="n">
-        <v>987262.9948789694</v>
+        <v>987262.9962853347</v>
       </c>
     </row>
     <row r="215">
@@ -2154,7 +2154,7 @@
         <v>1813</v>
       </c>
       <c r="B215" t="n">
-        <v>995478.3319825898</v>
+        <v>995478.3333802922</v>
       </c>
     </row>
     <row r="216">
@@ -2162,7 +2162,7 @@
         <v>1814</v>
       </c>
       <c r="B216" t="n">
-        <v>1003791.845168146</v>
+        <v>1003791.846556972</v>
       </c>
     </row>
     <row r="217">
@@ -2170,7 +2170,7 @@
         <v>1815</v>
       </c>
       <c r="B217" t="n">
-        <v>1012204.431997076</v>
+        <v>1012204.43337681</v>
       </c>
     </row>
     <row r="218">
@@ -2178,7 +2178,7 @@
         <v>1816</v>
       </c>
       <c r="B218" t="n">
-        <v>1020716.990871341</v>
+        <v>1020716.992241764</v>
       </c>
     </row>
     <row r="219">
@@ -2186,7 +2186,7 @@
         <v>1817</v>
       </c>
       <c r="B219" t="n">
-        <v>1029330.420805746</v>
+        <v>1029330.422166637</v>
       </c>
     </row>
     <row r="220">
@@ -2194,7 +2194,7 @@
         <v>1818</v>
       </c>
       <c r="B220" t="n">
-        <v>1038045.621193886</v>
+        <v>1038045.622545025</v>
       </c>
     </row>
     <row r="221">
@@ -2202,7 +2202,7 @@
         <v>1819</v>
       </c>
       <c r="B221" t="n">
-        <v>1046863.491567673</v>
+        <v>1046863.492908833</v>
       </c>
     </row>
     <row r="222">
@@ -2210,7 +2210,7 @@
         <v>1820</v>
       </c>
       <c r="B222" t="n">
-        <v>1055784.931350346</v>
+        <v>1055784.932681302</v>
       </c>
     </row>
     <row r="223">
@@ -2218,7 +2218,7 @@
         <v>1821</v>
       </c>
       <c r="B223" t="n">
-        <v>1064810.839602951</v>
+        <v>1064810.840923472</v>
       </c>
     </row>
     <row r="224">
@@ -2226,7 +2226,7 @@
         <v>1822</v>
       </c>
       <c r="B224" t="n">
-        <v>1073942.114764199</v>
+        <v>1073942.116074056</v>
       </c>
     </row>
     <row r="225">
@@ -2234,7 +2234,7 @@
         <v>1823</v>
       </c>
       <c r="B225" t="n">
-        <v>1083179.654383681</v>
+        <v>1083179.65568264</v>
       </c>
     </row>
     <row r="226">
@@ -2242,7 +2242,7 @@
         <v>1824</v>
       </c>
       <c r="B226" t="n">
-        <v>1092524.354848361</v>
+        <v>1092524.356136189</v>
       </c>
     </row>
     <row r="227">
@@ -2250,7 +2250,7 @@
         <v>1825</v>
       </c>
       <c r="B227" t="n">
-        <v>1101977.111102337</v>
+        <v>1101977.112378796</v>
       </c>
     </row>
     <row r="228">
@@ -2258,7 +2258,7 @@
         <v>1826</v>
       </c>
       <c r="B228" t="n">
-        <v>1111538.8163598</v>
+        <v>1111538.817624652</v>
       </c>
     </row>
     <row r="229">
@@ -2266,7 +2266,7 @@
         <v>1827</v>
       </c>
       <c r="B229" t="n">
-        <v>1121210.361811171</v>
+        <v>1121210.363064175</v>
       </c>
     </row>
     <row r="230">
@@ -2274,7 +2274,7 @@
         <v>1828</v>
       </c>
       <c r="B230" t="n">
-        <v>1130992.636322378</v>
+        <v>1130992.637563294</v>
       </c>
     </row>
     <row r="231">
@@ -2282,7 +2282,7 @@
         <v>1829</v>
       </c>
       <c r="B231" t="n">
-        <v>1140886.526127252</v>
+        <v>1140886.527355836</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>1830</v>
       </c>
       <c r="B232" t="n">
-        <v>1150892.914513008</v>
+        <v>1150892.915729014</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>1831</v>
       </c>
       <c r="B233" t="n">
-        <v>1161012.681498795</v>
+        <v>1161012.682701977</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>1832</v>
       </c>
       <c r="B234" t="n">
-        <v>1171246.703507316</v>
+        <v>1171246.704697425</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>1833</v>
       </c>
       <c r="B235" t="n">
-        <v>1181595.853029486</v>
+        <v>1181595.854206273</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>1834</v>
       </c>
       <c r="B236" t="n">
-        <v>1192060.998282144</v>
+        <v>1192060.999445359</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>1835</v>
       </c>
       <c r="B237" t="n">
-        <v>1202643.002858816</v>
+        <v>1202643.004008207</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>1836</v>
       </c>
       <c r="B238" t="n">
-        <v>1213342.725373531</v>
+        <v>1213342.726508844</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>1837</v>
       </c>
       <c r="B239" t="n">
-        <v>1224161.019097715</v>
+        <v>1224161.020218697</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>1838</v>
       </c>
       <c r="B240" t="n">
-        <v>1235098.731590182</v>
+        <v>1235098.732696577</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>1839</v>
       </c>
       <c r="B241" t="n">
-        <v>1246156.704320238</v>
+        <v>1246156.70541179</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>1840</v>
       </c>
       <c r="B242" t="n">
-        <v>1257335.772283949</v>
+        <v>1257335.773360402</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>1841</v>
       </c>
       <c r="B243" t="n">
-        <v>1268636.763613605</v>
+        <v>1268636.764674702</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>1842</v>
       </c>
       <c r="B244" t="n">
-        <v>1280060.499180426</v>
+        <v>1280060.500225909</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>1843</v>
       </c>
       <c r="B245" t="n">
-        <v>1291607.792190573</v>
+        <v>1291607.793220183</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>1844</v>
       </c>
       <c r="B246" t="n">
-        <v>1303279.44777452</v>
+        <v>1303279.448787997</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>1845</v>
       </c>
       <c r="B247" t="n">
-        <v>1315076.262569863</v>
+        <v>1315076.26356695</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>1846</v>
       </c>
       <c r="B248" t="n">
-        <v>1326999.024297647</v>
+        <v>1326999.025278084</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>1847</v>
       </c>
       <c r="B249" t="n">
-        <v>1339048.511332286</v>
+        <v>1339048.512295814</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>1848</v>
       </c>
       <c r="B250" t="n">
-        <v>1351225.492265189</v>
+        <v>1351225.49321155</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>1849</v>
       </c>
       <c r="B251" t="n">
-        <v>1363530.725462187</v>
+        <v>1363530.726391121</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>1850</v>
       </c>
       <c r="B252" t="n">
-        <v>1375964.958614866</v>
+        <v>1375964.959526114</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>1851</v>
       </c>
       <c r="B253" t="n">
-        <v>1388528.92828595</v>
+        <v>1388528.929179256</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>1852</v>
       </c>
       <c r="B254" t="n">
-        <v>1401223.359448847</v>
+        <v>1401223.360323952</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>1853</v>
       </c>
       <c r="B255" t="n">
-        <v>1414048.965021501</v>
+        <v>1414048.965878149</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>1854</v>
       </c>
       <c r="B256" t="n">
-        <v>1427006.445394713</v>
+        <v>1427006.446232648</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>1855</v>
       </c>
       <c r="B257" t="n">
-        <v>1440096.487955076</v>
+        <v>1440096.488774045</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>1856</v>
       </c>
       <c r="B258" t="n">
-        <v>1453319.766602707</v>
+        <v>1453319.767402455</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>1857</v>
       </c>
       <c r="B259" t="n">
-        <v>1466676.941263943</v>
+        <v>1466676.94204422</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>1858</v>
       </c>
       <c r="B260" t="n">
-        <v>1480168.657399211</v>
+        <v>1480168.658159765</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>1859</v>
       </c>
       <c r="B261" t="n">
-        <v>1493795.545506246</v>
+        <v>1493795.546246829</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>1860</v>
       </c>
       <c r="B262" t="n">
-        <v>1507558.220618902</v>
+        <v>1507558.221339267</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>1861</v>
       </c>
       <c r="B263" t="n">
-        <v>1521457.281801748</v>
+        <v>1521457.282501651</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>1862</v>
       </c>
       <c r="B264" t="n">
-        <v>1535493.311640698</v>
+        <v>1535493.312319896</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>1863</v>
       </c>
       <c r="B265" t="n">
-        <v>1549666.875729923</v>
+        <v>1549666.876388175</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>1864</v>
       </c>
       <c r="B266" t="n">
-        <v>1563978.522155282</v>
+        <v>1563978.522792351</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>1865</v>
       </c>
       <c r="B267" t="n">
-        <v>1578428.780974558</v>
+        <v>1578428.78159021</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>1866</v>
       </c>
       <c r="B268" t="n">
-        <v>1593018.163694768</v>
+        <v>1593018.16428877</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>1867</v>
       </c>
       <c r="B269" t="n">
-        <v>1607747.162746829</v>
+        <v>1607747.163318953</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>1868</v>
       </c>
       <c r="B270" t="n">
-        <v>1622616.250957893</v>
+        <v>1622616.251507914</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>1869</v>
       </c>
       <c r="B271" t="n">
-        <v>1637625.88102165</v>
+        <v>1637625.881549345</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>1870</v>
       </c>
       <c r="B272" t="n">
-        <v>1652776.484966931</v>
+        <v>1652776.485472083</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>1871</v>
       </c>
       <c r="B273" t="n">
-        <v>1668068.473624938</v>
+        <v>1668068.474107332</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>1872</v>
       </c>
       <c r="B274" t="n">
-        <v>1683502.236095443</v>
+        <v>1683502.23655487</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>1873</v>
       </c>
       <c r="B275" t="n">
-        <v>1699078.139212328</v>
+        <v>1699078.139648581</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>1874</v>
       </c>
       <c r="B276" t="n">
-        <v>1714796.527008808</v>
+        <v>1714796.527421686</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>1875</v>
       </c>
       <c r="B277" t="n">
-        <v>1730657.720182738</v>
+        <v>1730657.720572045</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>1876</v>
       </c>
       <c r="B278" t="n">
-        <v>1746662.015562377</v>
+        <v>1746662.015927921</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>1877</v>
       </c>
       <c r="B279" t="n">
-        <v>1762809.68557302</v>
+        <v>1762809.685914616</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>1878</v>
       </c>
       <c r="B280" t="n">
-        <v>1779100.9777049</v>
+        <v>1779100.978022366</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>1879</v>
       </c>
       <c r="B281" t="n">
-        <v>1795536.11398278</v>
+        <v>1795536.114275941</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>1880</v>
       </c>
       <c r="B282" t="n">
-        <v>1812115.290437677</v>
+        <v>1812115.290706364</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>1881</v>
       </c>
       <c r="B283" t="n">
-        <v>1828838.676581145</v>
+        <v>1828838.676825195</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>1882</v>
       </c>
       <c r="B284" t="n">
-        <v>1845706.414882577</v>
+        <v>1845706.415101833</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>1883</v>
       </c>
       <c r="B285" t="n">
-        <v>1862718.620249979</v>
+        <v>1862718.620444292</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>1884</v>
       </c>
       <c r="B286" t="n">
-        <v>1879875.379514698</v>
+        <v>1879875.379683924</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>1885</v>
       </c>
       <c r="B287" t="n">
-        <v>1897176.750920563</v>
+        <v>1897176.751064565</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>1886</v>
       </c>
       <c r="B288" t="n">
-        <v>1914622.763617944</v>
+        <v>1914622.763736594</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>1887</v>
       </c>
       <c r="B289" t="n">
-        <v>1932213.417163213</v>
+        <v>1932213.417256388</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>1888</v>
       </c>
       <c r="B290" t="n">
-        <v>1949948.681024116</v>
+        <v>1949948.681091703</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>1889</v>
       </c>
       <c r="B291" t="n">
-        <v>1967828.494091563</v>
+        <v>1967828.494133458</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>1890</v>
       </c>
       <c r="B292" t="n">
-        <v>1985852.764198354</v>
+        <v>1985852.764214458</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>1891</v>
       </c>
       <c r="B293" t="n">
-        <v>2004021.367645363</v>
+        <v>2004021.367635589</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>1892</v>
       </c>
       <c r="B294" t="n">
-        <v>2022334.148735717</v>
+        <v>2022334.148699983</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>1893</v>
       </c>
       <c r="B295" t="n">
-        <v>2040790.919317493</v>
+        <v>2040790.919255728</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>1894</v>
       </c>
       <c r="B296" t="n">
-        <v>2059391.458335484</v>
+        <v>2059391.458247627</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>1895</v>
       </c>
       <c r="B297" t="n">
-        <v>2078135.511392574</v>
+        <v>2078135.511278572</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>1896</v>
       </c>
       <c r="B298" t="n">
-        <v>2097022.790321272</v>
+        <v>2097022.790181082</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>1897</v>
       </c>
       <c r="B299" t="n">
-        <v>2116052.972765949</v>
+        <v>2116052.972599539</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>1898</v>
       </c>
       <c r="B300" t="n">
-        <v>2135225.701776345</v>
+        <v>2135225.701583693</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>1899</v>
       </c>
       <c r="B301" t="n">
-        <v>2154540.585412896</v>
+        <v>2154540.585193988</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>1900</v>
       </c>
       <c r="B302" t="n">
-        <v>2173997.196364421</v>
+        <v>2173997.196119258</v>
       </c>
     </row>
     <row r="303">
@@ -2858,7 +2858,7 @@
         <v>1901</v>
       </c>
       <c r="B303" t="n">
-        <v>2193595.071578763</v>
+        <v>2193595.071307354</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>1902</v>
       </c>
       <c r="B304" t="n">
-        <v>2213333.711906908</v>
+        <v>2213333.711609273</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>1903</v>
       </c>
       <c r="B305" t="n">
-        <v>2233212.581761144</v>
+        <v>2233212.581437316</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>1904</v>
       </c>
       <c r="B306" t="n">
-        <v>2253231.108787833</v>
+        <v>2253231.108437855</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>1905</v>
       </c>
       <c r="B307" t="n">
-        <v>2273388.683555323</v>
+        <v>2273388.683179252</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>1906</v>
       </c>
       <c r="B308" t="n">
-        <v>2293684.659257564</v>
+        <v>2293684.658855467</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>1907</v>
       </c>
       <c r="B309" t="n">
-        <v>2314118.351433958</v>
+        <v>2314118.351005916</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>1908</v>
       </c>
       <c r="B310" t="n">
-        <v>2334689.037706003</v>
+        <v>2334689.037252106</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>1909</v>
       </c>
       <c r="B311" t="n">
-        <v>2355395.957531231</v>
+        <v>2355395.957051586</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>1910</v>
       </c>
       <c r="B312" t="n">
-        <v>2376238.311974998</v>
+        <v>2376238.311469723</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>1911</v>
       </c>
       <c r="B313" t="n">
-        <v>2397215.263500625</v>
+        <v>2397215.262969852</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>1912</v>
       </c>
       <c r="B314" t="n">
-        <v>2418325.935778398</v>
+        <v>2418325.935222272</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>1913</v>
       </c>
       <c r="B315" t="n">
-        <v>2439569.413513935</v>
+        <v>2439569.412932614</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>1914</v>
       </c>
       <c r="B316" t="n">
-        <v>2460944.742296406</v>
+        <v>2460944.741690062</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>1915</v>
       </c>
       <c r="B317" t="n">
-        <v>2482450.928467073</v>
+        <v>2482450.927835892</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>1916</v>
       </c>
       <c r="B318" t="n">
-        <v>2504086.939008635</v>
+        <v>2504086.938352818</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>1917</v>
       </c>
       <c r="B319" t="n">
-        <v>2525851.701455809</v>
+        <v>2525851.70077557</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>1918</v>
       </c>
       <c r="B320" t="n">
-        <v>2547744.103827592</v>
+        <v>2547744.103123159</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>1919</v>
       </c>
       <c r="B321" t="n">
-        <v>2569762.994581629</v>
+        <v>2569762.993853247</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>1920</v>
       </c>
       <c r="B322" t="n">
-        <v>2591907.182591091</v>
+        <v>2591907.18183902</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>1921</v>
       </c>
       <c r="B323" t="n">
-        <v>2614175.437144452</v>
+        <v>2614175.436368962</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>1922</v>
       </c>
       <c r="B324" t="n">
-        <v>2636566.487968521</v>
+        <v>2636566.487169902</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>1923</v>
       </c>
       <c r="B325" t="n">
-        <v>2659079.025275113</v>
+        <v>2659079.02445367</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>1924</v>
       </c>
       <c r="B326" t="n">
-        <v>2681711.699831661</v>
+        <v>2681711.698987711</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>1925</v>
       </c>
       <c r="B327" t="n">
-        <v>2704463.123056091</v>
+        <v>2704463.12218997</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>1926</v>
       </c>
       <c r="B328" t="n">
-        <v>2727331.867136257</v>
+        <v>2727331.866248315</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>1927</v>
       </c>
       <c r="B329" t="n">
-        <v>2750316.465174193</v>
+        <v>2750316.464264795</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>1928</v>
       </c>
       <c r="B330" t="n">
-        <v>2773415.411355431</v>
+        <v>2773415.410424958</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>1929</v>
       </c>
       <c r="B331" t="n">
-        <v>2796627.161143607</v>
+        <v>2796627.160192458</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>1930</v>
       </c>
       <c r="B332" t="n">
-        <v>2819950.131500553</v>
+        <v>2819950.130529141</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>1931</v>
       </c>
       <c r="B333" t="n">
-        <v>2843382.701132033</v>
+        <v>2843382.700140788</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>1932</v>
       </c>
       <c r="B334" t="n">
-        <v>2866923.21075929</v>
+        <v>2866923.209748657</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>1933</v>
       </c>
       <c r="B335" t="n">
-        <v>2890569.963416499</v>
+        <v>2890569.962386938</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>1934</v>
       </c>
       <c r="B336" t="n">
-        <v>2914321.224774227</v>
+        <v>2914321.223726217</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>1935</v>
       </c>
       <c r="B337" t="n">
-        <v>2938175.223488969</v>
+        <v>2938175.222423006</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>1936</v>
       </c>
       <c r="B338" t="n">
-        <v>2962130.151578784</v>
+        <v>2962130.150495375</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>1937</v>
       </c>
       <c r="B339" t="n">
-        <v>2986184.164825027</v>
+        <v>2986184.163724699</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>1938</v>
       </c>
       <c r="B340" t="n">
-        <v>3010335.383200182</v>
+        <v>3010335.382083478</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>1939</v>
       </c>
       <c r="B341" t="n">
-        <v>3034581.891321711</v>
+        <v>3034581.89018919</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>1940</v>
       </c>
       <c r="B342" t="n">
-        <v>3058921.738931851</v>
+        <v>3058921.737784087</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>1941</v>
       </c>
       <c r="B343" t="n">
-        <v>3083352.941403234</v>
+        <v>3083352.940240819</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>1942</v>
       </c>
       <c r="B344" t="n">
-        <v>3107873.480270192</v>
+        <v>3107873.479093733</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>1943</v>
       </c>
       <c r="B345" t="n">
-        <v>3132481.303785567</v>
+        <v>3132481.302595685</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>1944</v>
       </c>
       <c r="B346" t="n">
-        <v>3157174.327502805</v>
+        <v>3157174.326300141</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>1945</v>
       </c>
       <c r="B347" t="n">
-        <v>3181950.434883118</v>
+        <v>3181950.433668325</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>1946</v>
       </c>
       <c r="B348" t="n">
-        <v>3206807.477927411</v>
+        <v>3206807.476701162</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>1947</v>
       </c>
       <c r="B349" t="n">
-        <v>3231743.277832706</v>
+        <v>3231743.276595684</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>1948</v>
       </c>
       <c r="B350" t="n">
-        <v>3256755.625672687</v>
+        <v>3256755.624425595</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>1949</v>
       </c>
       <c r="B351" t="n">
-        <v>3281842.283102042</v>
+        <v>3281842.281845596</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>1950</v>
       </c>
       <c r="B352" t="n">
-        <v>3307000.983084169</v>
+        <v>3307000.981819103</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>1951</v>
       </c>
       <c r="B353" t="n">
-        <v>3332229.430641844</v>
+        <v>3332229.429368904</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>1952</v>
       </c>
       <c r="B354" t="n">
-        <v>3357525.303630371</v>
+        <v>3357525.30235032</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>1953</v>
       </c>
       <c r="B355" t="n">
-        <v>3382886.253532741</v>
+        <v>3382886.252246355</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>1954</v>
       </c>
       <c r="B356" t="n">
-        <v>3408309.90627627</v>
+        <v>3408309.904984341</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>1955</v>
       </c>
       <c r="B357" t="n">
-        <v>3433793.863070174</v>
+        <v>3433793.861773507</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>1956</v>
       </c>
       <c r="B358" t="n">
-        <v>3459335.701263502</v>
+        <v>3459335.699962917</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>1957</v>
       </c>
       <c r="B359" t="n">
-        <v>3484932.975222815</v>
+        <v>3484932.973919145</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>1958</v>
       </c>
       <c r="B360" t="n">
-        <v>3510583.217228992</v>
+        <v>3510583.215923085</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>1959</v>
       </c>
       <c r="B361" t="n">
-        <v>3536283.938392486</v>
+        <v>3536283.937085204</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>1960</v>
       </c>
       <c r="B362" t="n">
-        <v>3562032.629586357</v>
+        <v>3562032.628278572</v>
       </c>
     </row>
     <row r="363">
@@ -3338,7 +3338,7 @@
         <v>1961</v>
       </c>
       <c r="B363" t="n">
-        <v>3587826.762396361</v>
+        <v>3587826.76108896</v>
       </c>
     </row>
     <row r="364">
@@ -3346,7 +3346,7 @@
         <v>1962</v>
       </c>
       <c r="B364" t="n">
-        <v>3613663.790087367</v>
+        <v>3613663.788781251</v>
       </c>
     </row>
     <row r="365">
@@ -3354,7 +3354,7 @@
         <v>1963</v>
       </c>
       <c r="B365" t="n">
-        <v>3639541.148585342</v>
+        <v>3639541.14728142</v>
       </c>
     </row>
     <row r="366">
@@ -3362,7 +3362,7 @@
         <v>1964</v>
       </c>
       <c r="B366" t="n">
-        <v>3665456.257474106</v>
+        <v>3665456.256173303</v>
       </c>
     </row>
     <row r="367">
@@ -3370,7 +3370,7 @@
         <v>1965</v>
       </c>
       <c r="B367" t="n">
-        <v>3691406.521006085</v>
+        <v>3691406.519709335</v>
       </c>
     </row>
     <row r="368">
@@ -3378,7 +3378,7 @@
         <v>1966</v>
       </c>
       <c r="B368" t="n">
-        <v>3717389.3291262</v>
+        <v>3717389.327834451</v>
       </c>
     </row>
     <row r="369">
@@ -3386,7 +3386,7 @@
         <v>1967</v>
       </c>
       <c r="B369" t="n">
-        <v>3743402.058508093</v>
+        <v>3743402.057222301</v>
       </c>
     </row>
     <row r="370">
@@ -3394,7 +3394,7 @@
         <v>1968</v>
       </c>
       <c r="B370" t="n">
-        <v>3769442.073601776</v>
+        <v>3769442.072322911</v>
       </c>
     </row>
     <row r="371">
@@ -3402,7 +3402,7 @@
         <v>1969</v>
       </c>
       <c r="B371" t="n">
-        <v>3795506.727691881</v>
+        <v>3795506.726420919</v>
       </c>
     </row>
     <row r="372">
@@ -3410,7 +3410,7 @@
         <v>1970</v>
       </c>
       <c r="B372" t="n">
-        <v>3821593.363965569</v>
+        <v>3821593.3627035</v>
       </c>
     </row>
     <row r="373">
@@ -3418,7 +3418,7 @@
         <v>1971</v>
       </c>
       <c r="B373" t="n">
-        <v>3847699.316589226</v>
+        <v>3847699.315337046</v>
       </c>
     </row>
     <row r="374">
@@ -3426,7 +3426,7 @@
         <v>1972</v>
       </c>
       <c r="B374" t="n">
-        <v>3873821.911792998</v>
+        <v>3873821.910551715</v>
       </c>
     </row>
     <row r="375">
@@ -3434,7 +3434,7 @@
         <v>1973</v>
       </c>
       <c r="B375" t="n">
-        <v>3899958.468962255</v>
+        <v>3899958.467732885</v>
       </c>
     </row>
     <row r="376">
@@ -3442,7 +3442,7 @@
         <v>1974</v>
       </c>
       <c r="B376" t="n">
-        <v>3926106.301735025</v>
+        <v>3926106.300518593</v>
       </c>
     </row>
     <row r="377">
@@ -3450,7 +3450,7 @@
         <v>1975</v>
       </c>
       <c r="B377" t="n">
-        <v>3952262.71910445</v>
+        <v>3952262.717901987</v>
       </c>
     </row>
     <row r="378">
@@ -3458,7 +3458,7 @@
         <v>1976</v>
       </c>
       <c r="B378" t="n">
-        <v>3978425.026525304</v>
+        <v>3978425.02533785</v>
       </c>
     </row>
     <row r="379">
@@ -3466,7 +3466,7 @@
         <v>1977</v>
       </c>
       <c r="B379" t="n">
-        <v>4004590.527023619</v>
+        <v>4004590.525852221</v>
       </c>
     </row>
     <row r="380">
@@ -3474,7 +3474,7 @@
         <v>1978</v>
       </c>
       <c r="B380" t="n">
-        <v>4030756.522308424</v>
+        <v>4030756.521154135</v>
       </c>
     </row>
     <row r="381">
@@ -3482,7 +3482,7 @@
         <v>1979</v>
       </c>
       <c r="B381" t="n">
-        <v>4056920.313884654</v>
+        <v>4056920.312748532</v>
       </c>
     </row>
     <row r="382">
@@ -3490,7 +3490,7 @@
         <v>1980</v>
       </c>
       <c r="B382" t="n">
-        <v>4083079.20416622</v>
+        <v>4083079.203049333</v>
       </c>
     </row>
     <row r="383">
@@ -3498,7 +3498,7 @@
         <v>1981</v>
       </c>
       <c r="B383" t="n">
-        <v>4109230.497588301</v>
+        <v>4109230.49649172</v>
       </c>
     </row>
     <row r="384">
@@ -3506,7 +3506,7 @@
         <v>1982</v>
       </c>
       <c r="B384" t="n">
-        <v>4135371.501717851</v>
+        <v>4135371.500642652</v>
       </c>
     </row>
     <row r="385">
@@ -3514,7 +3514,7 @@
         <v>1983</v>
       </c>
       <c r="B385" t="n">
-        <v>4161499.52836137</v>
+        <v>4161499.527308633</v>
       </c>
     </row>
     <row r="386">
@@ -3522,7 +3522,7 @@
         <v>1984</v>
       </c>
       <c r="B386" t="n">
-        <v>4187611.894668962</v>
+        <v>4187611.89363977</v>
       </c>
     </row>
     <row r="387">
@@ -3530,7 +3530,7 @@
         <v>1985</v>
       </c>
       <c r="B387" t="n">
-        <v>4213705.924233724</v>
+        <v>4213705.923229167</v>
       </c>
     </row>
     <row r="388">
@@ -3538,7 +3538,7 @@
         <v>1986</v>
       </c>
       <c r="B388" t="n">
-        <v>4239778.948185505</v>
+        <v>4239778.947206673</v>
       </c>
     </row>
     <row r="389">
@@ -3546,7 +3546,7 @@
         <v>1987</v>
       </c>
       <c r="B389" t="n">
-        <v>4265828.306278095</v>
+        <v>4265828.305326081</v>
       </c>
     </row>
     <row r="390">
@@ -3554,7 +3554,7 @@
         <v>1988</v>
       </c>
       <c r="B390" t="n">
-        <v>4291851.347968897</v>
+        <v>4291851.347044797</v>
       </c>
     </row>
     <row r="391">
@@ -3562,7 +3562,7 @@
         <v>1989</v>
       </c>
       <c r="B391" t="n">
-        <v>4317845.433490169</v>
+        <v>4317845.432595082</v>
       </c>
     </row>
     <row r="392">
@@ -3570,7 +3570,7 @@
         <v>1990</v>
       </c>
       <c r="B392" t="n">
-        <v>4343807.934910924</v>
+        <v>4343807.934045947</v>
       </c>
     </row>
     <row r="393">
@@ -3578,7 +3578,7 @@
         <v>1991</v>
       </c>
       <c r="B393" t="n">
-        <v>4369736.237188559</v>
+        <v>4369736.236354792</v>
       </c>
     </row>
     <row r="394">
@@ -3586,7 +3586,7 @@
         <v>1992</v>
       </c>
       <c r="B394" t="n">
-        <v>4395627.739209381</v>
+        <v>4395627.738407924</v>
       </c>
     </row>
     <row r="395">
@@ -3594,7 +3594,7 @@
         <v>1993</v>
       </c>
       <c r="B395" t="n">
-        <v>4421479.854817114</v>
+        <v>4421479.854049065</v>
       </c>
     </row>
     <row r="396">
@@ -3602,7 +3602,7 @@
         <v>1994</v>
       </c>
       <c r="B396" t="n">
-        <v>4447290.013828563</v>
+        <v>4447290.013095021</v>
       </c>
     </row>
     <row r="397">
@@ -3610,7 +3610,7 @@
         <v>1995</v>
       </c>
       <c r="B397" t="n">
-        <v>4473055.6630356</v>
+        <v>4473055.662337665</v>
       </c>
     </row>
     <row r="398">
@@ -3618,7 +3618,7 @@
         <v>1996</v>
       </c>
       <c r="B398" t="n">
-        <v>4498774.267192663</v>
+        <v>4498774.266531428</v>
       </c>
     </row>
     <row r="399">
@@ -3626,7 +3626,7 @@
         <v>1997</v>
       </c>
       <c r="B399" t="n">
-        <v>4524443.309988956</v>
+        <v>4524443.309365517</v>
       </c>
     </row>
     <row r="400">
@@ -3634,7 +3634,7 @@
         <v>1998</v>
       </c>
       <c r="B400" t="n">
-        <v>4550060.295004627</v>
+        <v>4550060.294420073</v>
       </c>
     </row>
     <row r="401">
@@ -3642,7 +3642,7 @@
         <v>1999</v>
       </c>
       <c r="B401" t="n">
-        <v>4575622.74665013</v>
+        <v>4575622.746105551</v>
       </c>
     </row>
     <row r="402">
@@ -3650,7 +3650,7 @@
         <v>2000</v>
       </c>
       <c r="B402" t="n">
-        <v>4601128.211088087</v>
+        <v>4601128.210584565</v>
       </c>
     </row>
     <row r="403">
@@ -3658,7 +3658,7 @@
         <v>2001</v>
       </c>
       <c r="B403" t="n">
-        <v>4626574.257136934</v>
+        <v>4626574.25667555</v>
       </c>
     </row>
     <row r="404">
@@ -3666,7 +3666,7 @@
         <v>2002</v>
       </c>
       <c r="B404" t="n">
-        <v>4651958.477155688</v>
+        <v>4651958.476737518</v>
       </c>
     </row>
     <row r="405">
@@ -3674,7 +3674,7 @@
         <v>2003</v>
       </c>
       <c r="B405" t="n">
-        <v>4677278.487909198</v>
+        <v>4677278.487535312</v>
       </c>
     </row>
     <row r="406">
@@ -3682,7 +3682,7 @@
         <v>2004</v>
       </c>
       <c r="B406" t="n">
-        <v>4702531.931413245</v>
+        <v>4702531.931084711</v>
       </c>
     </row>
     <row r="407">
@@ -3690,7 +3690,7 @@
         <v>2005</v>
       </c>
       <c r="B407" t="n">
-        <v>4727716.475758935</v>
+        <v>4727716.47547681</v>
       </c>
     </row>
     <row r="408">
@@ -3698,7 +3698,7 @@
         <v>2006</v>
       </c>
       <c r="B408" t="n">
-        <v>4752829.815915782</v>
+        <v>4752829.815681121</v>
       </c>
     </row>
     <row r="409">
@@ -3706,7 +3706,7 @@
         <v>2007</v>
       </c>
       <c r="B409" t="n">
-        <v>4777869.674513</v>
+        <v>4777869.674326848</v>
       </c>
     </row>
     <row r="410">
@@ -3714,7 +3714,7 @@
         <v>2008</v>
       </c>
       <c r="B410" t="n">
-        <v>4802833.802598461</v>
+        <v>4802833.80246186</v>
       </c>
     </row>
     <row r="411">
@@ -3722,7 +3722,7 @@
         <v>2009</v>
       </c>
       <c r="B411" t="n">
-        <v>4827719.980374879</v>
+        <v>4827719.980288858</v>
       </c>
     </row>
     <row r="412">
@@ -3730,7 +3730,7 @@
         <v>2010</v>
       </c>
       <c r="B412" t="n">
-        <v>4852526.017912762</v>
+        <v>4852526.017878346</v>
       </c>
     </row>
     <row r="413">
@@ -3738,7 +3738,7 @@
         <v>2011</v>
       </c>
       <c r="B413" t="n">
-        <v>4877249.755839731</v>
+        <v>4877249.755857934</v>
       </c>
     </row>
     <row r="414">
@@ -3746,7 +3746,7 @@
         <v>2012</v>
       </c>
       <c r="B414" t="n">
-        <v>4901889.066005826</v>
+        <v>4901889.066077656</v>
       </c>
     </row>
     <row r="415">
@@ -3754,7 +3754,7 @@
         <v>2013</v>
       </c>
       <c r="B415" t="n">
-        <v>4926441.85212446</v>
+        <v>4926441.852250914</v>
       </c>
     </row>
     <row r="416">
@@ -3762,7 +3762,7 @@
         <v>2014</v>
       </c>
       <c r="B416" t="n">
-        <v>4950906.050388689</v>
+        <v>4950906.050570753</v>
       </c>
     </row>
     <row r="417">
@@ -3770,7 +3770,7 @@
         <v>2015</v>
       </c>
       <c r="B417" t="n">
-        <v>4975279.630062529</v>
+        <v>4975279.630301181</v>
       </c>
     </row>
     <row r="418">
@@ -3778,7 +3778,7 @@
         <v>2016</v>
       </c>
       <c r="B418" t="n">
-        <v>4999560.594047066</v>
+        <v>4999560.594343274</v>
       </c>
     </row>
     <row r="419">
@@ -3786,7 +3786,7 @@
         <v>2017</v>
       </c>
       <c r="B419" t="n">
-        <v>5023746.979421135</v>
+        <v>5023746.979775855</v>
       </c>
     </row>
     <row r="420">
@@ -3794,7 +3794,7 @@
         <v>2018</v>
       </c>
       <c r="B420" t="n">
-        <v>5047836.857956378</v>
+        <v>5047836.858370554</v>
       </c>
     </row>
     <row r="421">
@@ -3802,7 +3802,7 @@
         <v>2019</v>
       </c>
       <c r="B421" t="n">
-        <v>5071828.336606519</v>
+        <v>5071828.337081086</v>
       </c>
     </row>
     <row r="422">
@@ -3810,7 +3810,7 @@
         <v>2020</v>
       </c>
       <c r="B422" t="n">
-        <v>5095719.557970755</v>
+        <v>5095719.558506633</v>
       </c>
     </row>
     <row r="423">
@@ -3818,7 +3818,7 @@
         <v>2021</v>
       </c>
       <c r="B423" t="n">
-        <v>5119508.700731117</v>
+        <v>5119508.701329217</v>
       </c>
     </row>
     <row r="424">
@@ -3826,7 +3826,7 @@
         <v>2022</v>
       </c>
       <c r="B424" t="n">
-        <v>5143193.980063793</v>
+        <v>5143193.980725012</v>
       </c>
     </row>
     <row r="425">
@@ -3834,7 +3834,7 @@
         <v>2023</v>
       </c>
       <c r="B425" t="n">
-        <v>5166773.648024329</v>
+        <v>5166773.64874955</v>
       </c>
     </row>
     <row r="426">
@@ -3842,7 +3842,7 @@
         <v>2024</v>
       </c>
       <c r="B426" t="n">
-        <v>5190245.993906733</v>
+        <v>5190245.994696828</v>
       </c>
     </row>
     <row r="427">
@@ -3850,7 +3850,7 @@
         <v>2025</v>
       </c>
       <c r="B427" t="n">
-        <v>5213609.34457649</v>
+        <v>5213609.345432317</v>
       </c>
     </row>
     <row r="428">
@@ -3858,7 +3858,7 @@
         <v>2026</v>
       </c>
       <c r="B428" t="n">
-        <v>5236862.064777547</v>
+        <v>5236862.065699951</v>
       </c>
     </row>
     <row r="429">
@@ -3866,7 +3866,7 @@
         <v>2027</v>
       </c>
       <c r="B429" t="n">
-        <v>5260002.557413346</v>
+        <v>5260002.558403155</v>
       </c>
     </row>
     <row r="430">
@@ -3874,7 +3874,7 @@
         <v>2028</v>
       </c>
       <c r="B430" t="n">
-        <v>5283029.263802006</v>
+        <v>5283029.264860035</v>
       </c>
     </row>
     <row r="431">
@@ -3882,7 +3882,7 @@
         <v>2029</v>
       </c>
       <c r="B431" t="n">
-        <v>5305940.663905802</v>
+        <v>5305940.665032855</v>
       </c>
     </row>
     <row r="432">
@@ -3890,7 +3890,7 @@
         <v>2030</v>
       </c>
       <c r="B432" t="n">
-        <v>5328735.276535101</v>
+        <v>5328735.277731963</v>
       </c>
     </row>
     <row r="433">
@@ -3898,7 +3898,7 @@
         <v>2031</v>
       </c>
       <c r="B433" t="n">
-        <v>5351411.65952692</v>
+        <v>5351411.660794363</v>
       </c>
     </row>
     <row r="434">
@@ -3906,7 +3906,7 @@
         <v>2032</v>
       </c>
       <c r="B434" t="n">
-        <v>5373968.409898346</v>
+        <v>5373968.411237128</v>
       </c>
     </row>
     <row r="435">
@@ -3914,7 +3914,7 @@
         <v>2033</v>
       </c>
       <c r="B435" t="n">
-        <v>5396404.163975046</v>
+        <v>5396404.165385907</v>
       </c>
     </row>
     <row r="436">
@@ -3922,7 +3922,7 @@
         <v>2034</v>
       </c>
       <c r="B436" t="n">
-        <v>5418717.597495104</v>
+        <v>5418717.59897877</v>
       </c>
     </row>
     <row r="437">
@@ -3930,7 +3930,7 @@
         <v>2035</v>
       </c>
       <c r="B437" t="n">
-        <v>5440907.425688514</v>
+        <v>5440907.427245693</v>
       </c>
     </row>
     <row r="438">
@@ -3938,7 +3938,7 @@
         <v>2036</v>
       </c>
       <c r="B438" t="n">
-        <v>5462972.403332571</v>
+        <v>5462972.404963958</v>
       </c>
     </row>
     <row r="439">
@@ -3946,7 +3946,7 @@
         <v>2037</v>
       </c>
       <c r="B439" t="n">
-        <v>5484911.324783544</v>
+        <v>5484911.326489818</v>
       </c>
     </row>
     <row r="440">
@@ -3954,7 +3954,7 @@
         <v>2038</v>
       </c>
       <c r="B440" t="n">
-        <v>5506723.023984942</v>
+        <v>5506723.025766764</v>
       </c>
     </row>
     <row r="441">
@@ -3962,7 +3962,7 @@
         <v>2039</v>
       </c>
       <c r="B441" t="n">
-        <v>5528406.374452735</v>
+        <v>5528406.37631075</v>
       </c>
     </row>
     <row r="442">
@@ -3970,7 +3970,7 @@
         <v>2040</v>
       </c>
       <c r="B442" t="n">
-        <v>5549960.289237935</v>
+        <v>5549960.291172772</v>
       </c>
     </row>
     <row r="443">
@@ -3978,7 +3978,7 @@
         <v>2041</v>
       </c>
       <c r="B443" t="n">
-        <v>5571383.720866916</v>
+        <v>5571383.722879186</v>
       </c>
     </row>
     <row r="444">
@@ -3986,7 +3986,7 @@
         <v>2042</v>
       </c>
       <c r="B444" t="n">
-        <v>5592675.661259896</v>
+        <v>5592675.663350195</v>
       </c>
     </row>
     <row r="445">
@@ -3994,7 +3994,7 @@
         <v>2043</v>
       </c>
       <c r="B445" t="n">
-        <v>5613835.141628015</v>
+        <v>5613835.143796923</v>
       </c>
     </row>
     <row r="446">
@@ -4002,7 +4002,7 @@
         <v>2044</v>
       </c>
       <c r="B446" t="n">
-        <v>5634861.232349454</v>
+        <v>5634861.234597531</v>
       </c>
     </row>
     <row r="447">
@@ -4010,7 +4010,7 @@
         <v>2045</v>
       </c>
       <c r="B447" t="n">
-        <v>5655753.042825053</v>
+        <v>5655753.045152843</v>
       </c>
     </row>
     <row r="448">
@@ -4018,7 +4018,7 @@
         <v>2046</v>
       </c>
       <c r="B448" t="n">
-        <v>5676509.721313891</v>
+        <v>5676509.723721922</v>
       </c>
     </row>
     <row r="449">
@@ -4026,7 +4026,7 @@
         <v>2047</v>
       </c>
       <c r="B449" t="n">
-        <v>5697130.454749346</v>
+        <v>5697130.457238129</v>
       </c>
     </row>
     <row r="450">
@@ -4034,7 +4034,7 @@
         <v>2048</v>
       </c>
       <c r="B450" t="n">
-        <v>5717614.468536085</v>
+        <v>5717614.471106113</v>
       </c>
     </row>
     <row r="451">
@@ -4042,7 +4042,7 @@
         <v>2049</v>
       </c>
       <c r="B451" t="n">
-        <v>5737961.026328521</v>
+        <v>5737961.02898027</v>
       </c>
     </row>
     <row r="452">
@@ -4050,7 +4050,7 @@
         <v>2050</v>
       </c>
       <c r="B452" t="n">
-        <v>5758169.429791242</v>
+        <v>5758169.432525172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>